<commit_message>
change for multi order
</commit_message>
<xml_diff>
--- a/src/assets/sample_shipments.xlsx
+++ b/src/assets/sample_shipments.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t xml:space="preserve">Weight</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t xml:space="preserve">External Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mode of Payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Split</t>
   </si>
   <si>
     <t xml:space="preserve">SHP12345</t>
@@ -86,6 +98,12 @@
     <t xml:space="preserve">PICKUP</t>
   </si>
   <si>
+    <t xml:space="preserve">try</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paid</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHP67890</t>
   </si>
   <si>
@@ -108,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">DROP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">again</t>
   </si>
 </sst>
 </file>
@@ -200,7 +221,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -231,6 +252,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -429,10 +454,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P15" activeCellId="0" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -483,87 +508,123 @@
       <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="9" t="n">
         <v>10.5</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>9877306965</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="8" t="n">
+        <v>24</v>
+      </c>
+      <c r="K2" s="9" t="n">
         <v>28.68</v>
       </c>
-      <c r="L2" s="8" t="n">
+      <c r="L2" s="9" t="n">
         <v>77.14</v>
       </c>
       <c r="M2" s="7" t="n">
         <v>1</v>
       </c>
+      <c r="N2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="n">
+      <c r="A3" s="10" t="n">
         <v>15</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>8977036927</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="8" t="n">
+        <v>34</v>
+      </c>
+      <c r="K3" s="9" t="n">
         <v>28.69</v>
       </c>
-      <c r="L3" s="8" t="n">
+      <c r="L3" s="9" t="n">
         <v>77.14</v>
       </c>
       <c r="M3" s="7" t="n">
         <v>3</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>